<commit_message>
Added custom sorting for class times
</commit_message>
<xml_diff>
--- a/public/New_Class_Data.xlsx
+++ b/public/New_Class_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CJ\Documents\My Projects\React_Practice\talium-schedule\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912183C5-6954-4E81-BB09-6E7804B01B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA800716-96EC-4D86-A3B2-54323CDB6631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9756" yWindow="264" windowWidth="13284" windowHeight="13416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>Blue | Purple | Red | Brown | Jr Black</t>
   </si>
   <si>
-    <t>No Belt  | White | Yellow | Orange</t>
-  </si>
-  <si>
     <t>SWAT Demo Team</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Day_Number</t>
+  </si>
+  <si>
+    <t>No Belt | White | Yellow | Orange</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -507,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A2:A48" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -545,11 +545,11 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -564,12 +564,12 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -593,11 +593,11 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -641,7 +641,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -665,11 +665,11 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -713,7 +713,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -737,7 +737,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -761,7 +761,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -785,7 +785,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -809,11 +809,11 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -828,12 +828,12 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="H14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -857,7 +857,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -881,7 +881,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -905,7 +905,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -929,7 +929,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -953,11 +953,11 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1001,11 +1001,11 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -1020,12 +1020,12 @@
         <v>0.70486111111111116</v>
       </c>
       <c r="H22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -1049,7 +1049,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1073,7 +1073,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -1097,7 +1097,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -1121,11 +1121,11 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1140,12 +1140,12 @@
         <v>0.78819444444444442</v>
       </c>
       <c r="H27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -1169,7 +1169,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -1193,7 +1193,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -1217,7 +1217,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -1241,11 +1241,11 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -1289,11 +1289,11 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
         <v>21</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -1337,11 +1337,11 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
         <v>21</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -1385,7 +1385,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -1409,11 +1409,11 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
         <v>21</v>
@@ -1433,11 +1433,11 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
         <v>21</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -1481,14 +1481,14 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -1505,14 +1505,14 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E43">
         <v>5</v>
@@ -1529,14 +1529,14 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E44">
         <v>5</v>
@@ -1553,14 +1553,14 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -1577,14 +1577,14 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" t="s">
         <v>25</v>
-      </c>
-      <c r="D46" t="s">
-        <v>26</v>
       </c>
       <c r="E46">
         <v>5</v>
@@ -1596,19 +1596,19 @@
         <v>0.78819444444444442</v>
       </c>
       <c r="H46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -1625,14 +1625,14 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E48">
         <v>5</v>

</xml_diff>